<commit_message>
AFDP-65 - Business Rules: Alfresco folder structure - updated business rules to set the CMIS path for a new complaint
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-complaint-plugin/src/main/resources/rules/drools-complaint-number-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-complaint-plugin/src/main/resources/rules/drools-complaint-number-rules.xlsx
@@ -17,12 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>RuleSet</t>
   </si>
   <si>
-    <t>Assign a Unique Complaint Number</t>
+    <t>Save Complaint Rules</t>
   </si>
   <si>
     <t>Import</t>
@@ -55,7 +55,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>RuleTable OPIS category folder rules</t>
+    <t>RuleTable Save Complaint Rules</t>
   </si>
   <si>
     <t>CONDITION</t>
@@ -70,7 +70,7 @@
     <t>$param == null</t>
   </si>
   <si>
-    <t>$complaint.setComplaintNumber($param);</t>
+    <t>$complaint.$1($2);</t>
   </si>
   <si>
     <t>If different rules apply to the same document, the last rule wins.</t>
@@ -91,7 +91,16 @@
     <t>complaintNumber</t>
   </si>
   <si>
-    <t>dateFormat('MM/dd/yyyy') + '_' + $complaint.getComplaintId()</t>
+    <t>setComplaintNumber, dateFormat('yyyyMMdd') + '_' + $complaint.getComplaintId()</t>
+  </si>
+  <si>
+    <t>Assign Alfresco Folder</t>
+  </si>
+  <si>
+    <t>ecmFolderId</t>
+  </si>
+  <si>
+    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Complaints/' + dateFormat('yyyyMMdd') + '_' + $complaint.getComplaintId()</t>
   </si>
 </sst>
 </file>
@@ -457,7 +466,7 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -465,7 +474,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4183673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="96.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="108.035714285714"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.5714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
   </cols>
@@ -604,9 +613,15 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
+      <c r="B16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>

</xml_diff>

<commit_message>
AFDP-892 - Store container folder IDs in a single shared table, not in columns in the container's table - convert Complaint module to use AcmContainerFolder
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-complaint-plugin/src/main/resources/rules/drools-complaint-number-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-complaint-plugin/src/main/resources/rules/drools-complaint-number-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="328" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -97,7 +97,7 @@
     <t>Assign Alfresco Folder</t>
   </si>
   <si>
-    <t>ecmFolderId</t>
+    <t>containerFolder.cmisFolderId</t>
   </si>
   <si>
     <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Complaints/' + dateFormat('yyyyMMdd') + '_' + $complaint.getComplaintId()</t>
@@ -108,7 +108,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -192,91 +192,91 @@
     </fill>
   </fills>
   <borders count="13">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
@@ -285,115 +285,115 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="6" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="7" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="8" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -465,8 +465,8 @@
   </sheetPr>
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -479,7 +479,7 @@
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -519,7 +519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -529,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8" t="s">
@@ -549,7 +549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
@@ -557,7 +557,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -567,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -575,7 +575,7 @@
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="11" t="s">
@@ -585,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="14">
       <c r="A14" s="13" t="s">
         <v>17</v>
       </c>
@@ -599,7 +599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -611,7 +611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="17" t="s">
         <v>24</v>
@@ -623,67 +623,67 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
       <c r="A17" s="1"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -692,7 +692,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -707,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -718,7 +718,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -733,8 +733,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,7 +744,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>